<commit_message>
modified:   package.json 	modified:   pnpm-lock.yaml 	new file:   prisma/migrations/20250311045227_add_kelas_to_assignment/migration.sql 	modified:   prisma/schema.prisma 	modified:   src/app/api/assignments/route.js 	modified:   src/app/api/auth/[...nextauth]/route.js 	modified:   src/app/api/register/route.js 	new file:   src/app/api/upload-tugas/route.js 	new file:   src/app/components/TugasTable.jsx 	modified:   src/app/globals.css 	modified:   src/app/layout.js 	deleted:    src/app/page.js 	new file:   src/app/page.jsx 	modified:   src/app/register/page.jsx 	modified:   src/app/server/rekap_files/rekap_tugas.xlsx 	modified:   src/app/server/server.js 	modified:   src/middleware.js
</commit_message>
<xml_diff>
--- a/src/app/server/rekap_files/rekap_tugas.xlsx
+++ b/src/app/server/rekap_files/rekap_tugas.xlsx
@@ -25,10 +25,10 @@
     <t>Link File</t>
   </si>
   <si>
-    <t>Budi</t>
-  </si>
-  <si>
-    <t>6281332218505</t>
+    <t>Adek</t>
+  </si>
+  <si>
+    <t>62895396334564</t>
   </si>
   <si>
     <t>Belum</t>

</xml_diff>

<commit_message>
modified:   src/app/components/TugasTable.jsx 	modified:   src/app/server/rekap_files/rekap_tugas.xlsx
</commit_message>
<xml_diff>
--- a/src/app/server/rekap_files/rekap_tugas.xlsx
+++ b/src/app/server/rekap_files/rekap_tugas.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>Nama</t>
   </si>
@@ -31,10 +31,28 @@
     <t>62895396334564</t>
   </si>
   <si>
+    <t>Sudah</t>
+  </si>
+  <si>
+    <t>"https://wgdxgzraacfhfbxvxuzy.supabase.co";/storage/v1/object/public/submissions/submissions/1742193980866.pdf</t>
+  </si>
+  <si>
+    <t>Budi</t>
+  </si>
+  <si>
+    <t>62895378394026</t>
+  </si>
+  <si>
     <t>Belum</t>
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Raka Tegar W</t>
+  </si>
+  <si>
+    <t>62895396334563</t>
   </si>
 </sst>
 </file>
@@ -411,7 +429,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -454,6 +472,34 @@
       </c>
       <c r="D3" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>